<commit_message>
push Co-authored-by: marcosgova777@gmail.com <marcosgova777@gmail.com>
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1.Archivos personales\5.University\2022-2023\Second quarter\IA\IA_project\IA_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D49D36-6867-4AAE-8DFB-359D60DE373D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260EB390-F365-49C5-936E-86DA7902CDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DCB117A6-A00E-404C-8D71-5719A07AB72F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>HEAT ON</t>
   </si>
@@ -103,12 +103,21 @@
   <si>
     <t>Column1</t>
   </si>
+  <si>
+    <t>Probabilities</t>
+  </si>
+  <si>
+    <t>COST ON</t>
+  </si>
+  <si>
+    <t>COST OFF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,16 +131,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -139,12 +169,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6438E2-D947-4732-BE0C-49D500C84AFF}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="73" workbookViewId="0">
-      <selection activeCell="Y44" sqref="Y44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="73" workbookViewId="0">
+      <selection activeCell="T57" sqref="T57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3023,13 +3068,251 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0.1666</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
+      <c r="C53" s="2">
+        <f>$A$50*1</f>
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="D53" s="2">
+        <f>$A$50*2</f>
+        <v>0.1666</v>
+      </c>
+      <c r="E53" s="2">
+        <f>$A$50*3</f>
+        <v>0.24990000000000001</v>
+      </c>
+      <c r="F53" s="2">
+        <f>$A$50*4</f>
+        <v>0.3332</v>
+      </c>
+      <c r="G53" s="2">
+        <f>$A$50*5</f>
+        <v>0.41649999999999998</v>
+      </c>
+      <c r="H53" s="2">
+        <f>$A$50*6</f>
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="I53" s="2">
+        <f>$A$50*7</f>
+        <v>0.58309999999999995</v>
+      </c>
+      <c r="J53" s="2">
+        <f>$A$50*8</f>
+        <v>0.66639999999999999</v>
+      </c>
+      <c r="K53" s="2">
+        <f>$A$50*9</f>
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="L53" s="2">
+        <f>$A$50*10</f>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="M53" s="2">
+        <f>$A$50*11</f>
+        <v>0.9163</v>
+      </c>
+      <c r="N53" s="2">
+        <f>$A$50*12</f>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="O53" s="2">
+        <f>$A$50*13</f>
+        <v>1.0829</v>
+      </c>
+      <c r="P53" s="2">
+        <f>$A$50*14</f>
+        <v>1.1661999999999999</v>
+      </c>
+      <c r="Q53" s="2">
+        <f>$A$50*15</f>
+        <v>1.2495000000000001</v>
+      </c>
+      <c r="R53" s="2">
+        <f>$A$50*16</f>
+        <v>1.3328</v>
+      </c>
+      <c r="S53" s="2">
+        <f>$A$50*17</f>
+        <v>1.4160999999999999</v>
+      </c>
+      <c r="T53" s="2">
+        <f>$A$50*18</f>
+        <v>1.4994000000000001</v>
+      </c>
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="1">
+        <f>$A$51*18</f>
+        <v>2.9988000000000001</v>
+      </c>
+      <c r="C54" s="1">
+        <f>$A$51*17</f>
+        <v>2.8321999999999998</v>
+      </c>
+      <c r="D54" s="1">
+        <f>$A$51*16</f>
+        <v>2.6656</v>
+      </c>
+      <c r="E54" s="1">
+        <f>$A$51*15</f>
+        <v>2.4990000000000001</v>
+      </c>
+      <c r="F54" s="1">
+        <f>$A$51*14</f>
+        <v>2.3323999999999998</v>
+      </c>
+      <c r="G54" s="1">
+        <f>$A$51*13</f>
+        <v>2.1657999999999999</v>
+      </c>
+      <c r="H54" s="1">
+        <f>$A$51*12</f>
+        <v>1.9992000000000001</v>
+      </c>
+      <c r="I54" s="1">
+        <f>$A$51*11</f>
+        <v>1.8326</v>
+      </c>
+      <c r="J54" s="1">
+        <f>$A$51*10</f>
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="K54" s="1">
+        <f>$A$51*9</f>
+        <v>1.4994000000000001</v>
+      </c>
+      <c r="L54" s="1">
+        <f>$A$51*8</f>
+        <v>1.3328</v>
+      </c>
+      <c r="M54" s="1">
+        <f>$A$51*7</f>
+        <v>1.1661999999999999</v>
+      </c>
+      <c r="N54" s="1">
+        <f>$A$51*6</f>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="O54" s="1">
+        <f>$A$51*5</f>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="P54" s="1">
+        <f>$A$51*4</f>
+        <v>0.66639999999999999</v>
+      </c>
+      <c r="Q54" s="1">
+        <f>$A$51*3</f>
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="R54" s="1">
+        <f>$A$51*2</f>
+        <v>0.3332</v>
+      </c>
+      <c r="S54" s="1">
+        <f>$A$51*1</f>
+        <v>0.1666</v>
+      </c>
+      <c r="T54" s="1">
+        <v>0</v>
+      </c>
+      <c r="U54" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="decimal" showInputMessage="1" showErrorMessage="1" sqref="B25:T43" xr:uid="{FFA6B623-A846-4069-9FBE-807E32835D02}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A52:U55" xr:uid="{E03A1E00-1EBE-4A57-9D69-9C004561EDC7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>